<commit_message>
Final Changes made for jenkin - Login
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="131">
   <si>
     <t>Environment Name</t>
   </si>
@@ -47,10 +47,10 @@
     <t>Login Screen Logo</t>
   </si>
   <si>
-    <t>Login Screen</t>
-  </si>
-  <si>
-    <t>HomePage</t>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Suite Page</t>
   </si>
   <si>
     <t>assets/img/xealei-logo2.png</t>
@@ -167,40 +167,61 @@
     <t>Suite</t>
   </si>
   <si>
+    <t>Carolina Farms</t>
+  </si>
+  <si>
+    <t>35.01</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>17.5632</t>
+  </si>
+  <si>
+    <t>Suite-22:14:55</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
     <t>Morrow Valley Farmstead</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Suite-07:51:00</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Suite-07:51:10</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Suite-07:51:21</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Suite-07:51:33</t>
+    <t>35.02</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>18.56327</t>
+  </si>
+  <si>
+    <t>Suite-22:15:08</t>
+  </si>
+  <si>
+    <t>35.03</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>19.5632</t>
+  </si>
+  <si>
+    <t>Suite-22:15:20</t>
+  </si>
+  <si>
+    <t>35.04</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>20.2415</t>
+  </si>
+  <si>
+    <t>Suite-22:15:35</t>
   </si>
   <si>
     <t>Breadth</t>
@@ -215,15 +236,9 @@
     <t>Royal</t>
   </si>
   <si>
-    <t>Carolina Farms</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -234,6 +249,204 @@
   </si>
   <si>
     <t>In-Active</t>
+  </si>
+  <si>
+    <t>Suite-22:35:56</t>
+  </si>
+  <si>
+    <t>Suite-22:36:06</t>
+  </si>
+  <si>
+    <t>Suite-22:36:18</t>
+  </si>
+  <si>
+    <t>Suite-22:38:16</t>
+  </si>
+  <si>
+    <t>Suite-22:38:27</t>
+  </si>
+  <si>
+    <t>Suite-22:38:39</t>
+  </si>
+  <si>
+    <t>Suite-22:38:53</t>
+  </si>
+  <si>
+    <t>Suite-22:47:58</t>
+  </si>
+  <si>
+    <t>Suite-22:51:15</t>
+  </si>
+  <si>
+    <t>Suite-22:51:26</t>
+  </si>
+  <si>
+    <t>Suite-22:51:39</t>
+  </si>
+  <si>
+    <t>Suite-23:06:01</t>
+  </si>
+  <si>
+    <t>Suite-23:06:11</t>
+  </si>
+  <si>
+    <t>Suite-23:06:23</t>
+  </si>
+  <si>
+    <t>Suite-23:06:36</t>
+  </si>
+  <si>
+    <t>Suite-23:10:58</t>
+  </si>
+  <si>
+    <t>Suite-23:17:41</t>
+  </si>
+  <si>
+    <t>Suite-23:17:53</t>
+  </si>
+  <si>
+    <t>Suite-23:18:04</t>
+  </si>
+  <si>
+    <t>Suite-23:18:17</t>
+  </si>
+  <si>
+    <t>Suite-23:22:48</t>
+  </si>
+  <si>
+    <t>Suite-23:23:00</t>
+  </si>
+  <si>
+    <t>Suite-23:23:20</t>
+  </si>
+  <si>
+    <t>Suite-23:23:34</t>
+  </si>
+  <si>
+    <t>Suite-08:29:13</t>
+  </si>
+  <si>
+    <t>Suite-08:31:27</t>
+  </si>
+  <si>
+    <t>Suite-08:32:03</t>
+  </si>
+  <si>
+    <t>Suite-08:32:14</t>
+  </si>
+  <si>
+    <t>Suite-08:32:25</t>
+  </si>
+  <si>
+    <t>Suite-08:32:37</t>
+  </si>
+  <si>
+    <t>Suite-08:41:06</t>
+  </si>
+  <si>
+    <t>Suite-08:41:16</t>
+  </si>
+  <si>
+    <t>Suite-08:41:27</t>
+  </si>
+  <si>
+    <t>Suite-08:41:38</t>
+  </si>
+  <si>
+    <t>Suite-09:08:44</t>
+  </si>
+  <si>
+    <t>Suite-09:08:53</t>
+  </si>
+  <si>
+    <t>Suite-09:09:05</t>
+  </si>
+  <si>
+    <t>Suite-09:09:16</t>
+  </si>
+  <si>
+    <t>Suite-09:16:36</t>
+  </si>
+  <si>
+    <t>Suite-09:16:45</t>
+  </si>
+  <si>
+    <t>Suite-09:21:01</t>
+  </si>
+  <si>
+    <t>Suite-09:21:11</t>
+  </si>
+  <si>
+    <t>Suite-09:21:23</t>
+  </si>
+  <si>
+    <t>Suite-09:21:34</t>
+  </si>
+  <si>
+    <t>Suite-09:26:58</t>
+  </si>
+  <si>
+    <t>Suite-09:27:08</t>
+  </si>
+  <si>
+    <t>Suite-09:27:20</t>
+  </si>
+  <si>
+    <t>Suite-09:27:31</t>
+  </si>
+  <si>
+    <t>Suite-09:35:00</t>
+  </si>
+  <si>
+    <t>Suite-09:35:10</t>
+  </si>
+  <si>
+    <t>Suite-09:35:21</t>
+  </si>
+  <si>
+    <t>Suite-09:35:32</t>
+  </si>
+  <si>
+    <t>Suite-09:48:41</t>
+  </si>
+  <si>
+    <t>Suite-09:51:37</t>
+  </si>
+  <si>
+    <t>Suite-09:55:09</t>
+  </si>
+  <si>
+    <t>Suite-09:57:23</t>
+  </si>
+  <si>
+    <t>Suite-09:58:00</t>
+  </si>
+  <si>
+    <t>Suite-09:58:10</t>
+  </si>
+  <si>
+    <t>Suite-09:58:20</t>
+  </si>
+  <si>
+    <t>Suite-09:58:32</t>
+  </si>
+  <si>
+    <t>Suite-10:38:35</t>
+  </si>
+  <si>
+    <t>Suite-10:41:08</t>
+  </si>
+  <si>
+    <t>Suite-10:41:52</t>
+  </si>
+  <si>
+    <t>Suite-10:42:02</t>
+  </si>
+  <si>
+    <t>Suite-10:42:18</t>
+  </si>
+  <si>
+    <t>Suite-10:42:31</t>
   </si>
 </sst>
 </file>
@@ -246,7 +459,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +497,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Comic Sans MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -828,137 +1047,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,41 +1200,49 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1339,44 +1566,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="29.0909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
+    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1395,30 +1622,30 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="24.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="14.2727272727273" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="24.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1443,75 +1670,75 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="16384" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="2" max="2" customWidth="true" width="34.0"/>
+    <col min="3" max="16384" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1532,18 +1759,18 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.6363636363636" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7272727272727" style="1" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7272727272727" customWidth="1"/>
-    <col min="8" max="16384" width="12.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.6363636363636"/>
+    <col min="2" max="2" customWidth="true" style="1" width="28.7272727272727"/>
+    <col min="3" max="5" customWidth="true" style="1" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" style="1" width="16.0"/>
+    <col min="7" max="7" customWidth="true" width="17.7272727272727"/>
+    <col min="8" max="16384" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="1" ht="18" spans="1:7">
@@ -1576,17 +1803,17 @@
       <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>42</v>
@@ -1596,20 +1823,20 @@
       <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="B3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>40</v>
+      <c r="C3" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>42</v>
@@ -1619,20 +1846,20 @@
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>40</v>
+      <c r="B4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>42</v>
@@ -1645,17 +1872,17 @@
       <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>40</v>
+      <c r="C5" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>42</v>
@@ -1678,10 +1905,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.3636363636364"/>
+    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
+    <col min="3" max="5" customWidth="true" style="1" width="12.9090909090909"/>
+    <col min="6" max="16384" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:7">
@@ -1695,44 +1922,44 @@
         <v>31</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>56</v>
+      <c r="E2" s="29" t="s">
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="7:7">
       <c r="G3" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suites > Add Suites Screen
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" activeTab="3"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Login" sheetId="2" r:id="rId3"/>
     <sheet name="AddSuites" sheetId="3" r:id="rId4"/>
     <sheet name="EditSuite" sheetId="4" r:id="rId5"/>
+    <sheet name="CreatedSuites" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="204">
   <si>
     <t>Environment Name</t>
   </si>
@@ -158,9 +159,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>CreatedSuite</t>
-  </si>
-  <si>
     <t>SuiteAvailability</t>
   </si>
   <si>
@@ -170,16 +168,13 @@
     <t>Carolina Farms</t>
   </si>
   <si>
-    <t>35.01</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>17.5632</t>
-  </si>
-  <si>
-    <t>Suite-22:14:55</t>
+    <t>30.01</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>30.5632</t>
   </si>
   <si>
     <t>Available</t>
@@ -188,57 +183,39 @@
     <t>Morrow Valley Farmstead</t>
   </si>
   <si>
-    <t>35.02</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>18.56327</t>
-  </si>
-  <si>
-    <t>Suite-22:15:08</t>
-  </si>
-  <si>
-    <t>35.03</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>19.5632</t>
-  </si>
-  <si>
-    <t>Suite-22:15:20</t>
-  </si>
-  <si>
-    <t>35.04</t>
+    <t>31</t>
+  </si>
+  <si>
+    <t>31.001</t>
+  </si>
+  <si>
+    <t>31.765</t>
+  </si>
+  <si>
+    <t>32.56327</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>32.56</t>
+  </si>
+  <si>
+    <t>Breadth</t>
+  </si>
+  <si>
+    <t>UpdatedSuite</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Royal</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>20.2415</t>
-  </si>
-  <si>
-    <t>Suite-22:15:35</t>
-  </si>
-  <si>
-    <t>Breadth</t>
-  </si>
-  <si>
-    <t>UpdatedSuite</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>Royal</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -251,202 +228,445 @@
     <t>In-Active</t>
   </si>
   <si>
-    <t>Suite-22:35:56</t>
-  </si>
-  <si>
-    <t>Suite-22:36:06</t>
-  </si>
-  <si>
-    <t>Suite-22:36:18</t>
-  </si>
-  <si>
-    <t>Suite-22:38:16</t>
-  </si>
-  <si>
-    <t>Suite-22:38:27</t>
-  </si>
-  <si>
-    <t>Suite-22:38:39</t>
-  </si>
-  <si>
-    <t>Suite-22:38:53</t>
-  </si>
-  <si>
-    <t>Suite-22:47:58</t>
-  </si>
-  <si>
-    <t>Suite-22:51:15</t>
-  </si>
-  <si>
-    <t>Suite-22:51:26</t>
-  </si>
-  <si>
-    <t>Suite-22:51:39</t>
-  </si>
-  <si>
-    <t>Suite-23:06:01</t>
-  </si>
-  <si>
-    <t>Suite-23:06:11</t>
-  </si>
-  <si>
-    <t>Suite-23:06:23</t>
-  </si>
-  <si>
-    <t>Suite-23:06:36</t>
-  </si>
-  <si>
-    <t>Suite-23:10:58</t>
-  </si>
-  <si>
-    <t>Suite-23:17:41</t>
-  </si>
-  <si>
-    <t>Suite-23:17:53</t>
-  </si>
-  <si>
-    <t>Suite-23:18:04</t>
-  </si>
-  <si>
-    <t>Suite-23:18:17</t>
-  </si>
-  <si>
-    <t>Suite-23:22:48</t>
-  </si>
-  <si>
-    <t>Suite-23:23:00</t>
-  </si>
-  <si>
-    <t>Suite-23:23:20</t>
-  </si>
-  <si>
-    <t>Suite-23:23:34</t>
-  </si>
-  <si>
-    <t>Suite-08:29:13</t>
-  </si>
-  <si>
-    <t>Suite-08:31:27</t>
-  </si>
-  <si>
-    <t>Suite-08:32:03</t>
-  </si>
-  <si>
-    <t>Suite-08:32:14</t>
-  </si>
-  <si>
-    <t>Suite-08:32:25</t>
-  </si>
-  <si>
-    <t>Suite-08:32:37</t>
-  </si>
-  <si>
-    <t>Suite-08:41:06</t>
-  </si>
-  <si>
-    <t>Suite-08:41:16</t>
-  </si>
-  <si>
-    <t>Suite-08:41:27</t>
-  </si>
-  <si>
-    <t>Suite-08:41:38</t>
-  </si>
-  <si>
-    <t>Suite-09:08:44</t>
-  </si>
-  <si>
-    <t>Suite-09:08:53</t>
-  </si>
-  <si>
-    <t>Suite-09:09:05</t>
-  </si>
-  <si>
-    <t>Suite-09:09:16</t>
-  </si>
-  <si>
-    <t>Suite-09:16:36</t>
-  </si>
-  <si>
-    <t>Suite-09:16:45</t>
-  </si>
-  <si>
-    <t>Suite-09:21:01</t>
-  </si>
-  <si>
-    <t>Suite-09:21:11</t>
-  </si>
-  <si>
-    <t>Suite-09:21:23</t>
-  </si>
-  <si>
-    <t>Suite-09:21:34</t>
-  </si>
-  <si>
-    <t>Suite-09:26:58</t>
-  </si>
-  <si>
-    <t>Suite-09:27:08</t>
-  </si>
-  <si>
-    <t>Suite-09:27:20</t>
-  </si>
-  <si>
-    <t>Suite-09:27:31</t>
-  </si>
-  <si>
-    <t>Suite-09:35:00</t>
-  </si>
-  <si>
-    <t>Suite-09:35:10</t>
-  </si>
-  <si>
-    <t>Suite-09:35:21</t>
-  </si>
-  <si>
-    <t>Suite-09:35:32</t>
-  </si>
-  <si>
-    <t>Suite-09:48:41</t>
-  </si>
-  <si>
-    <t>Suite-09:51:37</t>
-  </si>
-  <si>
-    <t>Suite-09:55:09</t>
-  </si>
-  <si>
-    <t>Suite-09:57:23</t>
-  </si>
-  <si>
-    <t>Suite-09:58:00</t>
-  </si>
-  <si>
-    <t>Suite-09:58:10</t>
-  </si>
-  <si>
-    <t>Suite-09:58:20</t>
-  </si>
-  <si>
-    <t>Suite-09:58:32</t>
-  </si>
-  <si>
-    <t>Suite-10:38:35</t>
-  </si>
-  <si>
-    <t>Suite-10:41:08</t>
-  </si>
-  <si>
-    <t>Suite-10:41:52</t>
-  </si>
-  <si>
-    <t>Suite-10:42:02</t>
-  </si>
-  <si>
-    <t>Suite-10:42:18</t>
-  </si>
-  <si>
-    <t>Suite-10:42:31</t>
+    <t>CreatedSuites</t>
+  </si>
+  <si>
+    <t>Suite-13:02:09</t>
+  </si>
+  <si>
+    <t>Suite-13:18:04</t>
+  </si>
+  <si>
+    <t>Suite-13:18:19</t>
+  </si>
+  <si>
+    <t>Suite-13:18:35</t>
+  </si>
+  <si>
+    <t>Suite-13:18:51</t>
+  </si>
+  <si>
+    <t>Suite-13:22:54</t>
+  </si>
+  <si>
+    <t>Suite-14:07:06</t>
+  </si>
+  <si>
+    <t>Suite-14:07:25</t>
+  </si>
+  <si>
+    <t>Suite-14:07:43</t>
+  </si>
+  <si>
+    <t>Suite-14:07:59</t>
+  </si>
+  <si>
+    <t>Suite-14:11:46</t>
+  </si>
+  <si>
+    <t>Suite-14:13:23</t>
+  </si>
+  <si>
+    <t>Suite-14:16:57</t>
+  </si>
+  <si>
+    <t>Suite-14:19:14</t>
+  </si>
+  <si>
+    <t>Suite-14:19:27</t>
+  </si>
+  <si>
+    <t>Suite-14:21:02</t>
+  </si>
+  <si>
+    <t>Suite-14:21:14</t>
+  </si>
+  <si>
+    <t>Suite-14:21:30</t>
+  </si>
+  <si>
+    <t>Suite-14:21:43</t>
+  </si>
+  <si>
+    <t>Suite-15:46:39</t>
+  </si>
+  <si>
+    <t>Suite-15:46:53</t>
+  </si>
+  <si>
+    <t>Suite-15:47:08</t>
+  </si>
+  <si>
+    <t>Suite-15:47:22</t>
+  </si>
+  <si>
+    <t>Suite-15:50:02</t>
+  </si>
+  <si>
+    <t>Suite-15:50:13</t>
+  </si>
+  <si>
+    <t>Suite-15:50:25</t>
+  </si>
+  <si>
+    <t>Suite-15:50:38</t>
+  </si>
+  <si>
+    <t>Suite-15:57:44</t>
+  </si>
+  <si>
+    <t>Suite-15:57:58</t>
+  </si>
+  <si>
+    <t>Suite-15:58:13</t>
+  </si>
+  <si>
+    <t>Suite-15:58:28</t>
+  </si>
+  <si>
+    <t>Suite-16:04:15</t>
+  </si>
+  <si>
+    <t>Suite-16:05:38</t>
+  </si>
+  <si>
+    <t>Suite-16:05:49</t>
+  </si>
+  <si>
+    <t>Suite-16:06:02</t>
+  </si>
+  <si>
+    <t>Suite-16:06:16</t>
+  </si>
+  <si>
+    <t>Suite-16:13:24</t>
+  </si>
+  <si>
+    <t>Suite-16:15:31</t>
+  </si>
+  <si>
+    <t>Suite-16:15:44</t>
+  </si>
+  <si>
+    <t>Suite-16:15:57</t>
+  </si>
+  <si>
+    <t>Suite-16:19:51</t>
+  </si>
+  <si>
+    <t>Suite-16:20:06</t>
+  </si>
+  <si>
+    <t>Suite-16:20:18</t>
+  </si>
+  <si>
+    <t>Suite-16:24:32</t>
+  </si>
+  <si>
+    <t>Suite-16:24:45</t>
+  </si>
+  <si>
+    <t>Suite-16:25:07</t>
+  </si>
+  <si>
+    <t>Suite-16:31:36</t>
+  </si>
+  <si>
+    <t>Suite-16:33:18</t>
+  </si>
+  <si>
+    <t>Suite-16:40:51</t>
+  </si>
+  <si>
+    <t>Suite-16:41:03</t>
+  </si>
+  <si>
+    <t>Suite-16:41:20</t>
+  </si>
+  <si>
+    <t>Suite-16:56:51</t>
+  </si>
+  <si>
+    <t>Suite-16:57:04</t>
+  </si>
+  <si>
+    <t>Suite-16:57:18</t>
+  </si>
+  <si>
+    <t>Suite-17:01:46</t>
+  </si>
+  <si>
+    <t>Suite-17:01:59</t>
+  </si>
+  <si>
+    <t>Suite-17:02:13</t>
+  </si>
+  <si>
+    <t>Suite-17:07:51</t>
+  </si>
+  <si>
+    <t>Suite-17:08:05</t>
+  </si>
+  <si>
+    <t>Suite-17:08:19</t>
+  </si>
+  <si>
+    <t>Suite-17:11:25</t>
+  </si>
+  <si>
+    <t>Suite-17:14:48</t>
+  </si>
+  <si>
+    <t>Suite-17:15:01</t>
+  </si>
+  <si>
+    <t>Suite-17:15:18</t>
+  </si>
+  <si>
+    <t>Suite-17:19:44</t>
+  </si>
+  <si>
+    <t>Suite-17:19:59</t>
+  </si>
+  <si>
+    <t>Suite-17:20:13</t>
+  </si>
+  <si>
+    <t>Suite-17:23:14</t>
+  </si>
+  <si>
+    <t>Suite-17:25:10</t>
+  </si>
+  <si>
+    <t>Suite-17:29:11</t>
+  </si>
+  <si>
+    <t>Suite-17:29:24</t>
+  </si>
+  <si>
+    <t>Suite-17:29:39</t>
+  </si>
+  <si>
+    <t>Suite-17:32:58</t>
+  </si>
+  <si>
+    <t>Suite-17:34:12</t>
+  </si>
+  <si>
+    <t>Suite-17:34:25</t>
+  </si>
+  <si>
+    <t>Suite-17:34:42</t>
+  </si>
+  <si>
+    <t>Suite-17:52:02</t>
+  </si>
+  <si>
+    <t>Suite-17:52:15</t>
+  </si>
+  <si>
+    <t>Suite-17:52:29</t>
+  </si>
+  <si>
+    <t>Suite-18:18:41</t>
+  </si>
+  <si>
+    <t>Suite-18:18:54</t>
+  </si>
+  <si>
+    <t>Suite-18:19:08</t>
+  </si>
+  <si>
+    <t>Suite-20:50:19</t>
+  </si>
+  <si>
+    <t>Suite-20:52:16</t>
+  </si>
+  <si>
+    <t>Suite-20:55:21</t>
+  </si>
+  <si>
+    <t>Suite-21:03:28</t>
+  </si>
+  <si>
+    <t>Suite-21:07:04</t>
+  </si>
+  <si>
+    <t>Suite-21:30:59</t>
+  </si>
+  <si>
+    <t>Suite-21:34:17</t>
+  </si>
+  <si>
+    <t>Suite-21:34:30</t>
+  </si>
+  <si>
+    <t>Suite-21:34:44</t>
+  </si>
+  <si>
+    <t>Suite-21:42:15</t>
+  </si>
+  <si>
+    <t>Suite-07:56:19</t>
+  </si>
+  <si>
+    <t>Suite-07:59:53</t>
+  </si>
+  <si>
+    <t>Suite-08:02:41</t>
+  </si>
+  <si>
+    <t>Suite-08:08:35</t>
+  </si>
+  <si>
+    <t>Suite-08:16:58</t>
+  </si>
+  <si>
+    <t>Suite-08:19:01</t>
+  </si>
+  <si>
+    <t>Suite-08:20:42</t>
+  </si>
+  <si>
+    <t>Suite-08:45:22</t>
+  </si>
+  <si>
+    <t>Suite-08:45:33</t>
+  </si>
+  <si>
+    <t>Suite-08:45:47</t>
+  </si>
+  <si>
+    <t>Suite-08:59:19</t>
+  </si>
+  <si>
+    <t>Suite-09:00:43</t>
+  </si>
+  <si>
+    <t>Suite-09:02:32</t>
+  </si>
+  <si>
+    <t>Suite-09:04:49</t>
+  </si>
+  <si>
+    <t>Suite-09:07:00</t>
+  </si>
+  <si>
+    <t>Suite-09:08:58</t>
+  </si>
+  <si>
+    <t>Suite-09:11:29</t>
+  </si>
+  <si>
+    <t>Suite-09:16:52</t>
+  </si>
+  <si>
+    <t>Suite-09:24:19</t>
+  </si>
+  <si>
+    <t>Suite-09:26:27</t>
+  </si>
+  <si>
+    <t>Suite-09:37:44</t>
+  </si>
+  <si>
+    <t>Suite-09:39:05</t>
+  </si>
+  <si>
+    <t>Suite-09:46:53</t>
+  </si>
+  <si>
+    <t>Suite-09:48:09</t>
+  </si>
+  <si>
+    <t>Suite-09:51:02</t>
+  </si>
+  <si>
+    <t>Suite-09:51:15</t>
+  </si>
+  <si>
+    <t>Suite-09:51:30</t>
+  </si>
+  <si>
+    <t>Suite-13:10:53</t>
+  </si>
+  <si>
+    <t>Suite-13:12:02</t>
+  </si>
+  <si>
+    <t>Suite-16:21:29</t>
+  </si>
+  <si>
+    <t>Suite-16:21:42</t>
+  </si>
+  <si>
+    <t>Suite-16:21:55</t>
+  </si>
+  <si>
+    <t>Suite-16:36:19</t>
+  </si>
+  <si>
+    <t>Suite-16:37:58</t>
+  </si>
+  <si>
+    <t>Suite-21:16:00</t>
+  </si>
+  <si>
+    <t>Suite-21:17:01</t>
+  </si>
+  <si>
+    <t>Suite-21:19:48</t>
+  </si>
+  <si>
+    <t>Suite-21:20:00</t>
+  </si>
+  <si>
+    <t>Suite-21:20:15</t>
+  </si>
+  <si>
+    <t>Suite-22:16:41</t>
+  </si>
+  <si>
+    <t>Suite-22:17:44</t>
+  </si>
+  <si>
+    <t>Suite-22:20:27</t>
+  </si>
+  <si>
+    <t>Suite-22:20:40</t>
+  </si>
+  <si>
+    <t>Suite-22:20:56</t>
+  </si>
+  <si>
+    <t>Suite-09:35:55</t>
+  </si>
+  <si>
+    <t>Suite-09:36:58</t>
+  </si>
+  <si>
+    <t>Suite-09:39:51</t>
+  </si>
+  <si>
+    <t>Suite-09:40:04</t>
+  </si>
+  <si>
+    <t>Suite-09:40:17</t>
+  </si>
+  <si>
+    <t>Suite-11:41:42</t>
+  </si>
+  <si>
+    <t>Suite-11:42:42</t>
+  </si>
+  <si>
+    <t>Suite-11:45:29</t>
+  </si>
+  <si>
+    <t>Suite-11:45:42</t>
+  </si>
+  <si>
+    <t>Suite-11:45:55</t>
   </si>
 </sst>
 </file>
@@ -469,6 +689,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF6A3E3E"/>
       <name val="Times New Roman"/>
@@ -504,14 +732,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1177,39 +1397,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1228,9 +1451,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1239,10 +1462,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1576,34 +1799,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1634,24 +1857,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1676,69 +1899,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1757,135 +1980,99 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.6363636363636"/>
-    <col min="2" max="2" customWidth="true" style="1" width="28.7272727272727"/>
-    <col min="3" max="5" customWidth="true" style="1" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" style="1" width="16.0"/>
-    <col min="7" max="7" customWidth="true" width="17.7272727272727"/>
-    <col min="8" max="16384" customWidth="true" width="12.6363636363636"/>
+    <col min="1" max="1" customWidth="true" style="2" width="12.6363636363636"/>
+    <col min="2" max="2" customWidth="true" style="2" width="28.7272727272727"/>
+    <col min="3" max="5" customWidth="true" style="2" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
+    <col min="7" max="16382" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="18" spans="1:7">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="12" customFormat="1" ht="18" spans="1:6">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="2" ht="15.5" spans="1:6">
+      <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="9" t="s">
+    </row>
+    <row r="3" ht="15.5" spans="1:6">
+      <c r="A3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" ht="15.5" spans="1:7">
-      <c r="A3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="D3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="F3" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" ht="15.5" spans="1:6">
+      <c r="A4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="15.5" spans="1:7">
-      <c r="A4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" ht="15.5" spans="1:7">
-      <c r="A5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>42</v>
+      <c r="E4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1900,66 +2087,831 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="12.3636363636364"/>
     <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
-    <col min="3" max="5" customWidth="true" style="1" width="12.9090909090909"/>
-    <col min="6" max="16384" customWidth="true" width="12.9090909090909"/>
+    <col min="3" max="5" customWidth="true" style="2" width="12.9090909090909"/>
+    <col min="6" max="16383" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" ht="15.5" spans="1:7">
+      <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="7:7">
+      <c r="G3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A149"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="27" t="s">
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="29" t="s">
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="7" t="s">
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="7:7">
-      <c r="G3" s="7" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pom4.xml MF Scenario Correction
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Environment Name</t>
   </si>
@@ -202,7 +202,15 @@
     <t>CreatedSuites</t>
   </si>
   <si>
-    <t>Suite-00:16:41</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SF-Pro-Display-Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Suite-08:45:12</t>
+    </r>
   </si>
   <si>
     <t>Created SuiteName</t>
@@ -211,22 +219,13 @@
     <t>Updated SuiteName</t>
   </si>
   <si>
-    <t>Suite-08:15:32</t>
-  </si>
-  <si>
-    <t>Royal-08:16:50</t>
-  </si>
-  <si>
-    <t>Royal-08:18:00</t>
-  </si>
-  <si>
-    <t>Suite-08:26:24</t>
-  </si>
-  <si>
-    <t>Royal-08:27:39</t>
-  </si>
-  <si>
-    <t>Royal-08:28:37</t>
+    <t>Suite-09:00:10</t>
+  </si>
+  <si>
+    <t>Royal-09:01:11</t>
+  </si>
+  <si>
+    <t>Royal-09:02:03</t>
   </si>
 </sst>
 </file>
@@ -256,9 +255,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="SF-Pro-Display-Regular"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1683,7 +1682,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1699,7 +1698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" ht="15.5" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
@@ -1717,21 +1716,6 @@
     <row r="5">
       <c r="A5" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1743,10 +1727,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -1779,22 +1763,6 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
TC1 & TC2 & TC3 - Completed
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Environment Name</t>
   </si>
@@ -34,7 +34,7 @@
     <t>https://qa.xealei.com/</t>
   </si>
   <si>
-    <t>PRE-POD</t>
+    <t>PRE-PROD</t>
   </si>
   <si>
     <t>https://preprod.xealei.com/</t>
@@ -206,66 +206,6 @@
   </si>
   <si>
     <t>Updated SuiteName</t>
-  </si>
-  <si>
-    <t>Suite-12:17:38</t>
-  </si>
-  <si>
-    <t>Suite-12:18:30</t>
-  </si>
-  <si>
-    <t>Suite-12:19:50</t>
-  </si>
-  <si>
-    <t>Suite-12:20:37</t>
-  </si>
-  <si>
-    <t>Suite-15:52:04</t>
-  </si>
-  <si>
-    <t>Suite-15:52:52</t>
-  </si>
-  <si>
-    <t>Suite-15:54:13</t>
-  </si>
-  <si>
-    <t>Suite-15:55:02</t>
-  </si>
-  <si>
-    <t>Suite-15:55:16</t>
-  </si>
-  <si>
-    <t>Suite-16:01:02</t>
-  </si>
-  <si>
-    <t>Royal-16:02:10</t>
-  </si>
-  <si>
-    <t>Royal-16:03:07</t>
-  </si>
-  <si>
-    <t>Suite-16:07:16</t>
-  </si>
-  <si>
-    <t>Suite-16:08:05</t>
-  </si>
-  <si>
-    <t>Suite-16:09:35</t>
-  </si>
-  <si>
-    <t>Suite-16:10:22</t>
-  </si>
-  <si>
-    <t>Suite-16:10:36</t>
-  </si>
-  <si>
-    <t>Suite-16:15:36</t>
-  </si>
-  <si>
-    <t>Royal-16:16:41</t>
-  </si>
-  <si>
-    <t>Royal-16:17:37</t>
   </si>
 </sst>
 </file>
@@ -976,7 +916,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1356,13 +1296,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
-    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
+    <col min="1" max="1" width="17.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="29.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1418,9 +1358,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="24.2727272727273"/>
-    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
+    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="24.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="14.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1460,9 +1400,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0"/>
-    <col min="2" max="2" customWidth="true" width="34.0"/>
-    <col min="3" max="16384" customWidth="true" width="18.0"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="16384" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1555,11 +1495,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="12.6363636363636"/>
-    <col min="2" max="2" customWidth="true" style="3" width="28.7272727272727"/>
-    <col min="3" max="5" customWidth="true" style="3" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
-    <col min="7" max="16382" customWidth="true" width="12.6363636363636"/>
+    <col min="1" max="1" width="12.6363636363636" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.7272727272727" style="3" customWidth="1"/>
+    <col min="3" max="5" width="12.6363636363636" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
+    <col min="7" max="16382" width="12.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="1" ht="18" spans="1:6">
@@ -1639,11 +1579,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0"/>
-    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
-    <col min="3" max="5" customWidth="true" style="3" width="12.9090909090909"/>
-    <col min="6" max="6" customWidth="true" width="25.7272727272727"/>
-    <col min="7" max="16379" customWidth="true" width="12.9090909090909"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
+    <col min="3" max="5" width="12.9090909090909" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.7272727272727" customWidth="1"/>
+    <col min="7" max="16379" width="12.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:6">
@@ -1715,135 +1655,20 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
+    <col min="1" max="1" width="22.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1855,16 +1680,16 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
-    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
+    <col min="1" max="1" width="18.0909090909091" customWidth="1"/>
+    <col min="2" max="2" width="22.4545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1875,38 +1700,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fix the error pom4.xml
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Environment Name</t>
   </si>
@@ -202,10 +202,22 @@
     <t>CreatedSuites</t>
   </si>
   <si>
+    <t>Suite-22:49:58</t>
+  </si>
+  <si>
     <t>Created SuiteName</t>
   </si>
   <si>
     <t>Updated SuiteName</t>
+  </si>
+  <si>
+    <t>Suite-23:40:49</t>
+  </si>
+  <si>
+    <t>Royal-23:42:05</t>
+  </si>
+  <si>
+    <t>Royal-23:43:04</t>
   </si>
 </sst>
 </file>
@@ -218,7 +230,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +245,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -786,157 +804,158 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,22 +964,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -968,7 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1301,39 +1320,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="29.0909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
+    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1358,9 +1377,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="24.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="14.2727272727273" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="24.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1375,13 +1394,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1400,75 +1419,75 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="16384" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="2" max="2" customWidth="true" width="34.0"/>
+    <col min="3" max="16384" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1495,70 +1514,70 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="12.6363636363636" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.7272727272727" style="3" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
-    <col min="7" max="16382" width="12.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="12.6363636363636"/>
+    <col min="2" max="2" customWidth="true" style="4" width="28.7272727272727"/>
+    <col min="3" max="5" customWidth="true" style="4" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
+    <col min="7" max="16382" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="18" spans="1:6">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="10" customFormat="1" ht="18" spans="1:6">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1579,70 +1598,70 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.7272727272727" customWidth="1"/>
-    <col min="7" max="16379" width="12.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.0"/>
+    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
+    <col min="3" max="5" customWidth="true" style="4" width="12.9090909090909"/>
+    <col min="6" max="6" customWidth="true" width="25.7272727272727"/>
+    <col min="7" max="16379" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1655,20 +1674,40 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="22.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1680,24 +1719,40 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="18.0909090909091" customWidth="1"/>
-    <col min="2" max="2" width="22.4545454545455" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
+    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>